<commit_message>
done what Rouven said
</commit_message>
<xml_diff>
--- a/tests/assets/excel_data.xlsx
+++ b/tests/assets/excel_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/RustroverProjects/PhenoXtrackt/tests/assets/pats_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/RustroverProjects/PhenoXtrackt/tests/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81794733-BA75-5F4E-946B-3A23641AD6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977ADEEC-19E4-4A4B-93C2-2DF7460CFEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="68800" windowHeight="28800" activeTab="1" xr2:uid="{B5F6743A-E238-884E-8FE8-3F2B7107E66E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="26600" xr2:uid="{B5F6743A-E238-884E-8FE8-3F2B7107E66E}"/>
   </bookViews>
   <sheets>
     <sheet name="basic info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>Patient ID</t>
   </si>
@@ -157,9 +157,6 @@
     <t>short stature</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>Lung abscess</t>
+  </si>
+  <si>
+    <t>P7Y5M8D</t>
   </si>
 </sst>
 </file>
@@ -245,7 +245,7 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5610DE-CD45-134C-8DD5-78D32384E21C}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,7 +615,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -629,7 +629,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -643,7 +643,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -656,12 +656,6 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
@@ -685,7 +679,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -703,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0072175-B97F-324E-BC6B-93A11147D02E}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -787,6 +781,9 @@
       </c>
       <c r="C4" t="s">
         <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
@@ -893,7 +890,7 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Remove "null" strings from test data
</commit_message>
<xml_diff>
--- a/tests/assets/excel_data.xlsx
+++ b/tests/assets/excel_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/RustroverProjects/PhenoXtrackt/tests/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rouvenreuter/Documents/Projects/PhenoXtrackt/tests/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977ADEEC-19E4-4A4B-93C2-2DF7460CFEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987622AA-DFF5-FA48-ABF5-0BEE14E61F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="26600" xr2:uid="{B5F6743A-E238-884E-8FE8-3F2B7107E66E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="26520" activeTab="2" xr2:uid="{B5F6743A-E238-884E-8FE8-3F2B7107E66E}"/>
   </bookViews>
   <sheets>
     <sheet name="basic info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Patient ID</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>bronchial Asthma</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>increased size of head</t>
@@ -584,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5610DE-CD45-134C-8DD5-78D32384E21C}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -615,7 +612,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -629,7 +626,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -643,7 +640,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -679,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -698,7 +695,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +734,7 @@
     </row>
     <row r="2" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -745,14 +742,11 @@
       <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -774,22 +768,22 @@
     </row>
     <row r="4" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.2">
@@ -816,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16582273-7520-304E-BE05-320B00A080F3}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,7 +850,7 @@
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -864,55 +858,40 @@
       <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
         <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
updated integration test with DOB and vital status details
</commit_message>
<xml_diff>
--- a/tests/assets/excel_data.xlsx
+++ b/tests/assets/excel_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/RustroverProjects/PhenoXtrackt/tests/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87426B8E-D798-524C-B76D-5B411FBA6A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25DA0E5-C4DB-6347-A0B8-14DFAD21A6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="26600" activeTab="2" xr2:uid="{B5F6743A-E238-884E-8FE8-3F2B7107E66E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="26600" xr2:uid="{B5F6743A-E238-884E-8FE8-3F2B7107E66E}"/>
   </bookViews>
   <sheets>
     <sheet name="basic info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Patient ID</t>
   </si>
@@ -173,6 +173,18 @@
   </si>
   <si>
     <t>Atrioseptal defect</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Time of death</t>
+  </si>
+  <si>
+    <t>P32Y</t>
+  </si>
+  <si>
+    <t>Survival time since diagnosis (days)</t>
   </si>
 </sst>
 </file>
@@ -242,12 +254,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,21 +597,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5610DE-CD45-134C-8DD5-78D32384E21C}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="3" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,10 +624,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -620,11 +646,14 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="5">
+        <v>20609</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -634,11 +663,20 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="7">
+        <v>123</v>
+      </c>
+      <c r="F3" s="5">
+        <v>31393</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -648,19 +686,25 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" s="5">
+        <v>38468</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" s="5">
+        <v>43905</v>
+      </c>
+      <c r="G5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -670,11 +714,11 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -684,7 +728,16 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5">
+        <v>45568</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1432</v>
+      </c>
+      <c r="F7" s="5">
+        <v>19040</v>
+      </c>
+      <c r="G7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -813,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16582273-7520-304E-BE05-320B00A080F3}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
+    <sheetView zoomScale="165" zoomScaleNormal="165" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated everything following our discussion
</commit_message>
<xml_diff>
--- a/tests/assets/excel_data.xlsx
+++ b/tests/assets/excel_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/RustroverProjects/PhenoXtrackt/tests/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BA929E-023B-D843-B9AE-DF15833F5FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDF6308-DCBA-1B41-9E89-7B5B40E1A697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="26600" activeTab="1" xr2:uid="{B5F6743A-E238-884E-8FE8-3F2B7107E66E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Patient ID</t>
   </si>
@@ -185,15 +185,6 @@
   </si>
   <si>
     <t>Survival time since diagnosis (days)</t>
-  </si>
-  <si>
-    <t>Rhinorrhea</t>
-  </si>
-  <si>
-    <t>HP:0012373</t>
-  </si>
-  <si>
-    <t>Date of onset</t>
   </si>
 </sst>
 </file>
@@ -755,10 +746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0072175-B97F-324E-BC6B-93A11147D02E}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,41 +840,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="5">
-        <v>35910</v>
-      </c>
-      <c r="C7" s="5">
-        <v>35910</v>
-      </c>
-      <c r="D7" s="5">
-        <v>44250</v>
-      </c>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G16" s="2"/>
@@ -891,17 +855,9 @@
     <row r="17" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G20" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>